<commit_message>
creaate One acc, paginate list acc
</commit_message>
<xml_diff>
--- a/backend/import.xlsx
+++ b/backend/import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tecinus/Desktop/Infinitea/SaleAccountTikTok/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6BAFF1-69C3-5D4D-93AB-F8463804A52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5DE549-EB9F-6A4D-BCDB-64A22FC6D298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="17500" xr2:uid="{3C2CC918-D297-CE4B-8CFC-4E794F16FAE7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3C2CC918-D297-CE4B-8CFC-4E794F16FAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,12 +46,6 @@
     <t>coin</t>
   </si>
   <si>
-    <t>qwerw</t>
-  </si>
-  <si>
-    <t>qwtwqt</t>
-  </si>
-  <si>
     <t>like</t>
   </si>
   <si>
@@ -73,34 +67,40 @@
     <t>link</t>
   </si>
   <si>
-    <t>ab231c@gmail.com</t>
-  </si>
-  <si>
-    <t>qw31231241ert@gmail.com</t>
-  </si>
-  <si>
-    <t>pfafffasoiis@gmail.com</t>
-  </si>
-  <si>
-    <t>ccs2131231so@gmail.con</t>
-  </si>
-  <si>
-    <t>po412424124141uqwro@hms.com</t>
-  </si>
-  <si>
-    <t>ab231c@gmaisl.com</t>
-  </si>
-  <si>
-    <t>qw31231241esrt@gmail.com</t>
-  </si>
-  <si>
-    <t>pfafffasoiis@gmafil.com</t>
-  </si>
-  <si>
-    <t>ccs213s1231so@gmail.con</t>
-  </si>
-  <si>
-    <t>po412424124141ffuqwro@hms.com</t>
+    <t>salwakhan2125@gmail.com</t>
+  </si>
+  <si>
+    <t>hg4fFvkdDfgg@</t>
+  </si>
+  <si>
+    <t>kumarsarvesh83641@gmail.com</t>
+  </si>
+  <si>
+    <t>hg8r6fIsKyyl@</t>
+  </si>
+  <si>
+    <t>hakamrahaman6767888@gmail.com</t>
+  </si>
+  <si>
+    <t>jasuwasanga09@gmail.com</t>
+  </si>
+  <si>
+    <t>OjcZviHzJMql@1</t>
+  </si>
+  <si>
+    <t>zeeshan645835@gmail.com</t>
+  </si>
+  <si>
+    <t>hg0miy2bNkmr@</t>
+  </si>
+  <si>
+    <t>sialshahid105@gmail.com</t>
+  </si>
+  <si>
+    <t>amirali03151075623@gmail.com</t>
+  </si>
+  <si>
+    <t>hg8a6gIoKtum@</t>
   </si>
 </sst>
 </file>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65E4387-B0C2-3F4C-AC77-C53037AB178B}">
-  <dimension ref="T1:AC11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,230 +506,203 @@
     <col min="21" max="21" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T2" s="3" t="s">
+      <c r="C2" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="1">
-        <v>123456</v>
-      </c>
-      <c r="V2" s="1">
-        <v>2234</v>
-      </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-    </row>
-    <row r="3" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="1">
-        <v>123456</v>
-      </c>
-      <c r="V3" s="1">
-        <v>4313</v>
-      </c>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T4" s="3" t="s">
+      <c r="C3" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="1">
-        <v>654321</v>
-      </c>
-      <c r="V4" s="1">
-        <v>2354</v>
-      </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T5" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V5" s="1">
-        <v>4215</v>
-      </c>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-    </row>
-    <row r="6" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T6" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V6" s="1">
-        <v>1234</v>
-      </c>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-    </row>
-    <row r="7" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T7" s="3" t="s">
+      <c r="C5" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="1">
-        <v>123456</v>
-      </c>
-      <c r="V7" s="1">
-        <v>1234</v>
-      </c>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-    </row>
-    <row r="8" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T8" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U8" s="1">
-        <v>123456</v>
-      </c>
-      <c r="V8" s="1">
-        <v>4313</v>
-      </c>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-    </row>
-    <row r="9" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T9" s="3" t="s">
+      <c r="C6" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U9" s="1">
-        <v>654321</v>
-      </c>
-      <c r="V9" s="1">
-        <v>2354</v>
-      </c>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-    </row>
-    <row r="10" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T10" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V10" s="1">
-        <v>4215</v>
-      </c>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-    </row>
-    <row r="11" spans="20:29" x14ac:dyDescent="0.2">
-      <c r="T11" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="V11" s="1">
-        <v>1234</v>
-      </c>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
+      <c r="C8" s="1">
+        <v>7000</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{7F6C9DD8-3DCC-A942-90CB-646D65D3501D}"/>
-    <hyperlink ref="T3" r:id="rId2" xr:uid="{DEBEE7A1-576B-0146-B357-8F8801CF10FE}"/>
-    <hyperlink ref="T4" r:id="rId3" xr:uid="{19BEBB0D-216F-2147-91A9-F8120035DCF8}"/>
-    <hyperlink ref="T5" r:id="rId4" xr:uid="{A8A419DC-7E0A-824D-B15A-108F1B80F06D}"/>
-    <hyperlink ref="T6" r:id="rId5" xr:uid="{95F0643A-571E-1643-9389-98D8DB844088}"/>
-    <hyperlink ref="T7" r:id="rId6" xr:uid="{D30652C9-9FD9-2D42-9409-883EE6E75ECC}"/>
-    <hyperlink ref="T8" r:id="rId7" xr:uid="{8B63ADE9-F078-C14B-9DEF-706FCC97B496}"/>
-    <hyperlink ref="T9" r:id="rId8" xr:uid="{76699B86-6D79-DF4D-8B4A-42023DE9611F}"/>
-    <hyperlink ref="T10" r:id="rId9" xr:uid="{930AFD03-9779-C341-A92E-79C39B355868}"/>
-    <hyperlink ref="T11" r:id="rId10" xr:uid="{65476E47-E352-B249-BE11-BE1E5488A27C}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{6877315A-9FEE-534E-9D4E-D1F08505D4CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>